<commit_message>
8-7-18 O: drive upload
</commit_message>
<xml_diff>
--- a/Bundling List for Mark.xlsx
+++ b/Bundling List for Mark.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18225" windowHeight="12210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lesson 1" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson 2" sheetId="2" r:id="rId2"/>
     <sheet name="Lesson 3" sheetId="3" r:id="rId3"/>
     <sheet name="Lesson 4" sheetId="4" r:id="rId4"/>
-    <sheet name="For Mark - Consolitated" sheetId="5" r:id="rId5"/>
+    <sheet name="Lesson 5" sheetId="7" r:id="rId5"/>
+    <sheet name="Shared Materials" sheetId="8" r:id="rId6"/>
+    <sheet name="For Mark - Consolitated" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t xml:space="preserve">Materials To Be Bundled </t>
   </si>
@@ -75,9 +77,6 @@
     <t>Webstaurant</t>
   </si>
   <si>
-    <t>11 bags per club. Bundled however is easiest.</t>
-  </si>
-  <si>
     <t>Comes in boxes of 250 bags</t>
   </si>
   <si>
@@ -94,13 +93,220 @@
   </si>
   <si>
     <t>Comes in case of 100 pans</t>
+  </si>
+  <si>
+    <t>Lesson 5</t>
+  </si>
+  <si>
+    <t>11 bags per club. 10 bags rolled inside of 1 bag will work.</t>
+  </si>
+  <si>
+    <t>Shared Materials</t>
+  </si>
+  <si>
+    <t>3 oz. paper cups</t>
+  </si>
+  <si>
+    <t>webstaurant</t>
+  </si>
+  <si>
+    <t>100 cups/club. In a bag, taped together, etc. whatever is best!</t>
+  </si>
+  <si>
+    <t>Cup Catcher Bag</t>
+  </si>
+  <si>
+    <t>Amazon (thread, pongs), Oriental Trading (duct tape, balloons)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each Bag Contains: invisible thread, 2 Turquiose latex balloons, 2 ping pong balls, 1 rainbow duct tape, 2-16 oz. clear cups (Teen Interns have pre-holed) </t>
+  </si>
+  <si>
+    <t>Each Bag Contains: invisible thread, 2 Turquiose latex balloons, 2 ping pong balls, 1 rainbow duct tape, 2 (Teen Interns have pre-holed) 16 oz. clear cups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These bags will NOT be in bin or curbside. One bag/site will be given to educators with binders at training. We will assemble these in training. These materials will be an "in-hand" material at training. </t>
+  </si>
+  <si>
+    <t>Soup Spoons</t>
+  </si>
+  <si>
+    <t>Bundle in a bag</t>
+  </si>
+  <si>
+    <t>110 bundles of 25 spoons. RA also needs spoons, maybe bundle together?</t>
+  </si>
+  <si>
+    <t>IN BIN</t>
+  </si>
+  <si>
+    <t>Toy Bags (Pop-Up Spring Toys, Boinks, and Pullback Cars)</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a bag </t>
+  </si>
+  <si>
+    <t>Bag of 30 Toys (10 Pop-Up Spring Toys, 10 pullback racers, 10 Boinks) Per Club</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110 Bags Total </t>
+  </si>
+  <si>
+    <t>Ping Pong Balls</t>
+  </si>
+  <si>
+    <t>110 sets</t>
+  </si>
+  <si>
+    <t>10" Cardboard Sheets</t>
+  </si>
+  <si>
+    <t>ULINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tied together would probably be the best. I guess that can be taped, AS LONG AS the tape does not ruin the surface of the cardboard. </t>
+  </si>
+  <si>
+    <t>110 Sets</t>
+  </si>
+  <si>
+    <t>Wooden Spools &amp; Velcro Strips</t>
+  </si>
+  <si>
+    <t>Amazon and ULINE</t>
+  </si>
+  <si>
+    <t>25 spools &amp; 25 strip sets (set=hook and loop strips)</t>
+  </si>
+  <si>
+    <t>110 Bags</t>
+  </si>
+  <si>
+    <t>Deli Containers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stacked and taped? </t>
+  </si>
+  <si>
+    <t>110 sets of 50 containers</t>
+  </si>
+  <si>
+    <t>AT TRAINING, GIVE WITH BINDER / NOT IN BIN</t>
+  </si>
+  <si>
+    <t>Glow Bags-</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 pkg </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> glow Powder</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1 pkg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> green </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>glow Powder</t>
+    </r>
+  </si>
+  <si>
+    <t>3- 4 oz Bottles of White Glue</t>
+  </si>
+  <si>
+    <t>Dollar Tree</t>
+  </si>
+  <si>
+    <t>5- Mixing paint trays</t>
+  </si>
+  <si>
+    <t>5 Pipettes</t>
+  </si>
+  <si>
+    <r>
+      <t>1 pkg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> blue </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Glow Powder</t>
+    </r>
+  </si>
+  <si>
+    <t>All 6 Items in a bag</t>
+  </si>
+  <si>
+    <t>Diffraction Grating Peepholes</t>
+  </si>
+  <si>
+    <t>Rainbow Symphony</t>
+  </si>
+  <si>
+    <t>Bag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am not sure how hey will come packaged, if not already bundled in 25. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +383,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -219,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,6 +481,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +765,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F6"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +774,7 @@
     <col min="3" max="3" width="62" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="40.5703125" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -572,61 +807,145 @@
       </c>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="4">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4">
+        <v>50</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1053,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1383,7 @@
     <col min="3" max="3" width="62.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -1104,31 +1424,31 @@
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -1350,7 +1670,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection sqref="A1:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,6 +1912,545 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="4">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4">
+        <v>100</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>